<commit_message>
Driver Script Oct 17
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Live_8oclock\hybrid_FrameWork\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8E7A1D-6271-4719-B50F-7331E766C9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15678DB6-DBF2-491C-83EB-C8A29F624D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8890" yWindow="0" windowWidth="10310" windowHeight="10080" firstSheet="1" activeTab="1" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
+    <workbookView xWindow="8890" yWindow="0" windowWidth="10310" windowHeight="10080" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618BA786-C995-4156-AC99-F1585CDFC29D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DBDB48-8853-497E-BE74-D35B630D87C1}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
driver script oct 18
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Live_8oclock\hybrid_FrameWork\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15678DB6-DBF2-491C-83EB-C8A29F624D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9138B4-C4AC-4B36-BF6F-378ADCAED2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8890" yWindow="0" windowWidth="10310" windowHeight="10080" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -182,6 +182,120 @@
   </si>
   <si>
     <t>validate page title</t>
+  </si>
+  <si>
+    <t>Click Stock items link</t>
+  </si>
+  <si>
+    <t>//a[text()='Stock Items ']</t>
+  </si>
+  <si>
+    <t>Wait for stock item</t>
+  </si>
+  <si>
+    <t>Wait for add Icon</t>
+  </si>
+  <si>
+    <t>Click Add icon</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t>Select item in Category</t>
+  </si>
+  <si>
+    <t>dropDownAction</t>
+  </si>
+  <si>
+    <t>Selct item in Supplier Number</t>
+  </si>
+  <si>
+    <t>x_Category</t>
+  </si>
+  <si>
+    <t>//select[@id='x_Category']</t>
+  </si>
+  <si>
+    <t>x_Supplier_Number</t>
+  </si>
+  <si>
+    <t>Captue Stock number</t>
+  </si>
+  <si>
+    <t>captureStock</t>
+  </si>
+  <si>
+    <t>Enter Stock name</t>
+  </si>
+  <si>
+    <t>Puzzels</t>
+  </si>
+  <si>
+    <t>x_Stock_Name</t>
+  </si>
+  <si>
+    <t>Select item in Unit Measurement</t>
+  </si>
+  <si>
+    <t>Enter Purchasing Price</t>
+  </si>
+  <si>
+    <t>Enter selling price</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Selling Puzzles</t>
+  </si>
+  <si>
+    <t>x_Unit_Of_Measurement</t>
+  </si>
+  <si>
+    <t>x_Purchasing_Price</t>
+  </si>
+  <si>
+    <t>x_Selling_Price</t>
+  </si>
+  <si>
+    <t>x_Notes</t>
+  </si>
+  <si>
+    <t>Click add button</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>Verify Stock Number</t>
+  </si>
+  <si>
+    <t>stockTable</t>
+  </si>
+  <si>
+    <t>Wait for Category Listbox</t>
+  </si>
+  <si>
+    <t>Wait for Confirm ok button</t>
+  </si>
+  <si>
+    <t>Click Confirm ok button</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>Wait for alert ok</t>
+  </si>
+  <si>
+    <t>Click Alert ok</t>
+  </si>
+  <si>
+    <t>(//button[starts-with(text(),'OK')])[6]</t>
+  </si>
+  <si>
+    <t>//input[@name='x_Stock_Number']</t>
   </si>
 </sst>
 </file>
@@ -260,12 +374,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618BA786-C995-4156-AC99-F1585CDFC29D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -614,7 +730,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -626,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -664,7 +780,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A10" sqref="A10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,40 +999,559 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5EABFA-4036-4B38-9829-CE9D260951EE}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="1">
+        <v>300000</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="1">
+        <v>500000</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="3">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="3">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hybrid driver script oct 19
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Live_8oclock\hybrid_FrameWork\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9138B4-C4AC-4B36-BF6F-378ADCAED2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0319D2A-A09E-42C4-BDD4-6E902A972CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{0E5B0FCA-BF53-4C30-B51D-9F8D03E66D7C}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="137">
   <si>
     <t>TCID</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>ExecutionStatus</t>
   </si>
   <si>
@@ -296,13 +293,169 @@
   </si>
   <si>
     <t>//input[@name='x_Stock_Number']</t>
+  </si>
+  <si>
+    <t>Wait for Supplier link</t>
+  </si>
+  <si>
+    <t>(//a[starts-with(text(),'Suppliers')])[2]</t>
+  </si>
+  <si>
+    <t>Click Supplier link</t>
+  </si>
+  <si>
+    <t>capturesup</t>
+  </si>
+  <si>
+    <t>Wait for Supplier Number</t>
+  </si>
+  <si>
+    <t>capture supplier number</t>
+  </si>
+  <si>
+    <t>Enter supplier name</t>
+  </si>
+  <si>
+    <t>Enter address</t>
+  </si>
+  <si>
+    <t>Enter City</t>
+  </si>
+  <si>
+    <t>Enter Country</t>
+  </si>
+  <si>
+    <t>Enter phone number</t>
+  </si>
+  <si>
+    <t>Enter Email</t>
+  </si>
+  <si>
+    <t>Enter Mobile number</t>
+  </si>
+  <si>
+    <t>Enter Notes</t>
+  </si>
+  <si>
+    <t>Click Add bytton</t>
+  </si>
+  <si>
+    <t>Enter Contact person</t>
+  </si>
+  <si>
+    <t>Verify Supplier number</t>
+  </si>
+  <si>
+    <t>suppliertable</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Supplier_Name']</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Address']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_City']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Country']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Contact_Person']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Phone_Number']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Mobile_Number']</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Notes']</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>Ameerpet,201,flat,beside satyam</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>QedgeTech</t>
+  </si>
+  <si>
+    <t>6872897652</t>
+  </si>
+  <si>
+    <t>Test@gmail.com</t>
+  </si>
+  <si>
+    <t>Iam Supplying Ig goods</t>
+  </si>
+  <si>
+    <t>capture Customer number</t>
+  </si>
+  <si>
+    <t>Wait for Customer Number</t>
+  </si>
+  <si>
+    <t>Enter Customer name</t>
+  </si>
+  <si>
+    <t>Wait for Customer link</t>
+  </si>
+  <si>
+    <t>Click Customer link</t>
+  </si>
+  <si>
+    <t>capturecus</t>
+  </si>
+  <si>
+    <t>(//a[contains(text(),'Customers')])[2]</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Customer_Name']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Notes']</t>
+  </si>
+  <si>
+    <t>Ranga</t>
+  </si>
+  <si>
+    <t>alwal</t>
+  </si>
+  <si>
+    <t>secunderabad</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Iam Customer</t>
+  </si>
+  <si>
+    <t>Click Add button</t>
+  </si>
+  <si>
+    <t>customertable</t>
+  </si>
+  <si>
+    <t>//input[@id='x__Email']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Customer_Number']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +484,14 @@
       <color rgb="FF231917"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,10 +532,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -382,8 +544,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -699,7 +870,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -730,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -754,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -766,7 +937,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -794,19 +965,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -814,52 +985,52 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="3">
         <v>10</v>
@@ -868,70 +1039,70 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3">
         <v>10</v>
@@ -940,55 +1111,55 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -1001,9 +1172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5EABFA-4036-4B38-9829-CE9D260951EE}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,19 +1188,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
@@ -1037,52 +1208,52 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="3">
         <v>10</v>
@@ -1091,70 +1262,70 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3">
         <v>10</v>
@@ -1163,34 +1334,34 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
@@ -1199,84 +1370,88 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1285,16 +1460,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1303,52 +1478,52 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -1357,16 +1532,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1">
         <v>300000</v>
@@ -1375,16 +1550,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1">
         <v>500000</v>
@@ -1393,52 +1568,52 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="3">
         <v>10</v>
@@ -1447,34 +1622,34 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="3">
         <v>10</v>
@@ -1483,73 +1658,73 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1560,84 +1735,1208 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C836F748-4684-4158-8E1B-B8DC4A171496}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="9">
+        <v>6882927682</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="3">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="3">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{9F2EF2F4-1F3A-4B9F-AE2B-3F5F28B7E055}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEB9B7B-CA62-4713-9EE2-D16BEF6F0B77}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="10">
+        <v>748374184</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="9">
+        <v>254524555</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="3">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="3">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{A286A81F-DC72-410E-80A3-E44A106BD789}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>